<commit_message>
Scrum for Sprint 3
</commit_message>
<xml_diff>
--- a/Scrum/Milestone 3/Sprint 3 Backlog.xlsx
+++ b/Scrum/Milestone 3/Sprint 3 Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\Desktop\SEPT\Scrum\Milestone 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142267DB-AEF0-4C76-B226-DA14AD9D08D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC40DFD-F0C3-462E-A57E-60899D41C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,502 +500,7 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <fill>
         <patternFill>
@@ -2043,7 +1548,7 @@
   <dimension ref="B1:J43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2124,10 +1629,10 @@
         <v>14</v>
       </c>
       <c r="G5" s="25"/>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="20"/>
+      <c r="I5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="20"/>
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2143,10 +1648,10 @@
         <v>14</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="20"/>
+      <c r="I6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="20"/>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2162,10 +1667,10 @@
         <v>14</v>
       </c>
       <c r="G7" s="25"/>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="20"/>
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
@@ -2185,10 +1690,10 @@
         <v>13</v>
       </c>
       <c r="G8" s="21"/>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="20"/>
+      <c r="I8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="20"/>
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2204,10 +1709,10 @@
         <v>13</v>
       </c>
       <c r="G9" s="21"/>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="20"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2223,10 +1728,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="21"/>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="20"/>
+      <c r="I10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="20"/>
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="2:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
@@ -2246,10 +1751,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="21"/>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="20"/>
+      <c r="I11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="20"/>
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2265,10 +1770,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="21"/>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="20"/>
+      <c r="I12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="20"/>
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2284,10 +1789,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="21"/>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="20"/>
+      <c r="I13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="20"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
@@ -2307,10 +1812,10 @@
         <v>14</v>
       </c>
       <c r="G14" s="21"/>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="20"/>
+      <c r="I14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="20"/>
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2326,10 +1831,10 @@
         <v>14</v>
       </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="20"/>
+      <c r="I15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="20"/>
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2345,10 +1850,10 @@
         <v>14</v>
       </c>
       <c r="G16" s="21"/>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="20"/>
+      <c r="I16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="20"/>
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="2:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
@@ -2368,10 +1873,10 @@
         <v>14</v>
       </c>
       <c r="G17" s="21"/>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="20"/>
+      <c r="I17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="20"/>
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2387,10 +1892,10 @@
         <v>14</v>
       </c>
       <c r="G18" s="21"/>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="20"/>
+      <c r="I18" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="20"/>
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
@@ -2406,10 +1911,10 @@
         <v>14</v>
       </c>
       <c r="G19" s="21"/>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="20"/>
+      <c r="I19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="20"/>
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="2:10" ht="25.5" x14ac:dyDescent="0.3">
@@ -2429,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="G20" s="21"/>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="20"/>
+      <c r="I20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="20"/>
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
@@ -2448,10 +1953,10 @@
         <v>9</v>
       </c>
       <c r="G21" s="21"/>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="20"/>
+      <c r="I21" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="20"/>
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
@@ -2467,10 +1972,10 @@
         <v>9</v>
       </c>
       <c r="G22" s="21"/>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="20"/>
+      <c r="I22" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="20"/>
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="2:10" ht="25.5" x14ac:dyDescent="0.3">
@@ -2490,10 +1995,10 @@
         <v>9</v>
       </c>
       <c r="G23" s="21"/>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="20"/>
+      <c r="I23" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="20"/>
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
@@ -2509,10 +2014,10 @@
         <v>9</v>
       </c>
       <c r="G24" s="21"/>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="20"/>
+      <c r="I24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="20"/>
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
@@ -2528,10 +2033,10 @@
         <v>9</v>
       </c>
       <c r="G25" s="21"/>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="20"/>
+      <c r="I25" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="20"/>
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="2:10" ht="25.5" x14ac:dyDescent="0.3">
@@ -2551,10 +2056,10 @@
         <v>9</v>
       </c>
       <c r="G26" s="21"/>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="20"/>
+      <c r="I26" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="20"/>
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
@@ -2570,10 +2075,10 @@
         <v>9</v>
       </c>
       <c r="G27" s="21"/>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="20"/>
+      <c r="I27" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="20"/>
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
@@ -2589,10 +2094,10 @@
         <v>9</v>
       </c>
       <c r="G28" s="21"/>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="20"/>
+      <c r="I28" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="20"/>
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
@@ -2612,10 +2117,10 @@
         <v>12</v>
       </c>
       <c r="G29" s="21"/>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="20"/>
+      <c r="I29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I29" s="20"/>
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
@@ -2631,10 +2136,10 @@
         <v>12</v>
       </c>
       <c r="G30" s="21"/>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="20"/>
+      <c r="I30" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="20"/>
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
@@ -2650,10 +2155,10 @@
         <v>12</v>
       </c>
       <c r="G31" s="21"/>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="20"/>
+      <c r="I31" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="20"/>
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
@@ -2673,10 +2178,10 @@
         <v>12</v>
       </c>
       <c r="G32" s="21"/>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="20"/>
+      <c r="I32" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I32" s="20"/>
       <c r="J32" s="16"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
@@ -2692,10 +2197,10 @@
         <v>12</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="20" t="s">
+      <c r="H33" s="20"/>
+      <c r="I33" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I33" s="20"/>
       <c r="J33" s="14"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
@@ -2711,10 +2216,10 @@
         <v>12</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="20"/>
+      <c r="I34" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="20"/>
       <c r="J34" s="14"/>
     </row>
     <row r="35" spans="2:10" ht="25.5" x14ac:dyDescent="0.3">
@@ -2734,10 +2239,10 @@
         <v>9</v>
       </c>
       <c r="G35" s="21"/>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="20"/>
+      <c r="I35" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I35" s="20"/>
       <c r="J35" s="14"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
@@ -2753,10 +2258,10 @@
         <v>9</v>
       </c>
       <c r="G36" s="21"/>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="20"/>
+      <c r="I36" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="20"/>
       <c r="J36" s="14"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
@@ -2772,10 +2277,10 @@
         <v>9</v>
       </c>
       <c r="G37" s="21"/>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="20"/>
+      <c r="I37" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="20"/>
       <c r="J37" s="14"/>
     </row>
     <row r="38" spans="2:10" ht="25.5" x14ac:dyDescent="0.3">
@@ -2795,10 +2300,10 @@
         <v>11</v>
       </c>
       <c r="G38" s="21"/>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="20"/>
+      <c r="I38" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="20"/>
       <c r="J38" s="14"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
@@ -2814,10 +2319,10 @@
         <v>11</v>
       </c>
       <c r="G39" s="21"/>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="20"/>
+      <c r="I39" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="20"/>
       <c r="J39" s="14"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
@@ -2833,10 +2338,10 @@
         <v>11</v>
       </c>
       <c r="G40" s="21"/>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="20"/>
+      <c r="I40" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="20"/>
       <c r="J40" s="14"/>
     </row>
     <row r="41" spans="2:10" ht="25.5" x14ac:dyDescent="0.3">
@@ -2856,10 +2361,10 @@
         <v>14</v>
       </c>
       <c r="G41" s="21"/>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="20"/>
+      <c r="I41" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="20"/>
       <c r="J41" s="14"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
@@ -2875,10 +2380,10 @@
         <v>14</v>
       </c>
       <c r="G42" s="21"/>
-      <c r="H42" s="20" t="s">
+      <c r="H42" s="20"/>
+      <c r="I42" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="20"/>
       <c r="J42" s="14"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
@@ -2894,155 +2399,155 @@
         <v>14</v>
       </c>
       <c r="G43" s="21"/>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="20"/>
+      <c r="I43" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="20"/>
       <c r="J43" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B33:D34 C27:D28 B27:D27 B9:C10 C30:D31 E9:E10 B12:E13 B15:E16 B18:E19 B21:E22 G26:G32 G12:G22 G9:G10 B5 F5:G5 J5:J32 H5:I43 D5 B6:G7">
-    <cfRule type="expression" dxfId="83" priority="113">
+  <conditionalFormatting sqref="B33:D34 C27:D28 B27:D27 B9:C10 C30:D31 E9:E10 B12:E13 B15:E16 B18:E19 B21:E22 G26:G32 G12:G22 G9:G10 B5 F5:G5 J5:J32 D5 B6:G7 H5:I43">
+    <cfRule type="expression" dxfId="50" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G34">
-    <cfRule type="expression" dxfId="82" priority="99">
+    <cfRule type="expression" dxfId="49" priority="99">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:J42">
-    <cfRule type="expression" dxfId="81" priority="97">
+    <cfRule type="expression" dxfId="48" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43">
-    <cfRule type="expression" dxfId="79" priority="94">
+    <cfRule type="expression" dxfId="47" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28 B30:B31">
-    <cfRule type="expression" dxfId="78" priority="93">
+    <cfRule type="expression" dxfId="46" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G7 B9:C9 E9 D9:D10 G9 B8:D8 F8:G8 F9:F10">
-    <cfRule type="expression" dxfId="77" priority="85">
+    <cfRule type="expression" dxfId="45" priority="85">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="76" priority="84">
+    <cfRule type="expression" dxfId="44" priority="84">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:G6 B5 F5:G5 D5 F6:F7">
-    <cfRule type="expression" dxfId="75" priority="82">
+    <cfRule type="expression" dxfId="43" priority="82">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:D40 B42:D43 B35:D37 F35:G37 G38:G43">
-    <cfRule type="expression" dxfId="74" priority="81">
+    <cfRule type="expression" dxfId="42" priority="81">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D25 G23:G25">
-    <cfRule type="expression" dxfId="72" priority="78">
+    <cfRule type="expression" dxfId="41" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="expression" dxfId="71" priority="77">
+    <cfRule type="expression" dxfId="40" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11 F11:G11 D11 F12:F13">
-    <cfRule type="expression" dxfId="70" priority="76">
+    <cfRule type="expression" dxfId="39" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11 F11:G11 D11 F12:F13">
-    <cfRule type="expression" dxfId="69" priority="75">
+    <cfRule type="expression" dxfId="38" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14 D14 F14:F19">
-    <cfRule type="expression" dxfId="68" priority="74">
+    <cfRule type="expression" dxfId="37" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17 D17">
-    <cfRule type="expression" dxfId="67" priority="73">
+    <cfRule type="expression" dxfId="36" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20 D20 F20:F28">
-    <cfRule type="expression" dxfId="66" priority="72">
+    <cfRule type="expression" dxfId="35" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23 D23">
-    <cfRule type="expression" dxfId="65" priority="71">
+    <cfRule type="expression" dxfId="34" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26 D26">
-    <cfRule type="expression" dxfId="64" priority="70">
+    <cfRule type="expression" dxfId="33" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 D29 F29:F34">
-    <cfRule type="expression" dxfId="63" priority="69">
+    <cfRule type="expression" dxfId="32" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32 D32">
-    <cfRule type="expression" dxfId="62" priority="68">
+    <cfRule type="expression" dxfId="31" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38:D38 F38:F40">
-    <cfRule type="expression" dxfId="58" priority="64">
+    <cfRule type="expression" dxfId="30" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:D41 F41:F43">
-    <cfRule type="expression" dxfId="57" priority="63">
+    <cfRule type="expression" dxfId="29" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E25">
-    <cfRule type="expression" dxfId="36" priority="39">
+    <cfRule type="expression" dxfId="28" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:E28">
-    <cfRule type="expression" dxfId="35" priority="38">
+    <cfRule type="expression" dxfId="27" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="26" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E34">
-    <cfRule type="expression" dxfId="33" priority="36">
+    <cfRule type="expression" dxfId="25" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E37">
-    <cfRule type="expression" dxfId="32" priority="35">
+    <cfRule type="expression" dxfId="24" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E40">
-    <cfRule type="expression" dxfId="31" priority="34">
+    <cfRule type="expression" dxfId="23" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E43">
-    <cfRule type="expression" dxfId="30" priority="33">
+    <cfRule type="expression" dxfId="22" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4200,9 +3705,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4378,19 +3886,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C82FB4F2-286A-40A1-8011-220F672FEF88}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E11F8907-776F-44AD-B681-425AE9F3D166}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4414,9 +3918,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E11F8907-776F-44AD-B681-425AE9F3D166}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C82FB4F2-286A-40A1-8011-220F672FEF88}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>